<commit_message>
Updated ECE to EEE | excel
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617446C9-C9F8-4109-BAFA-465580A2BB17}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" firstSheet="15" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" tabRatio="1000" firstSheet="10" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="8" r:id="rId1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="383">
   <si>
     <t>lecturer_id</t>
   </si>
@@ -262,9 +263,6 @@
     <t>Et nulla magna dolore aute duis dolore ex ex sit ullamco consequat non in id id laborum duis ea aute dolor incididunt do labore nisi anim sed nisi dolor dolore labore ea dolor in incididunt aute esse enim sunt esse sit in laborum aute consequat esse velit consequat cupidatat id voluptate dolor excepteur incididunt anim reprehenderit cillum dolore consequat aute sunt esse minim in excepteur ut culpa pariatur nulla culpa excepteur nisi ut aute aute nulla ad deserunt excepteur amet ex eu ea do enim amet deserunt aliqua pariatur veniam adipisicing ullamco incididunt amet consectetur do amet esse pariatur mollit in qui veniam ex dolore eu id dolore sunt in in aute veniam eiusmod in exercitation mollit fugiat duis minim incididunt commodo veniam sint sit amet anim veniam pariatur ad sunt quis re</t>
   </si>
   <si>
-    <t>ECE</t>
-  </si>
-  <si>
     <t>lecturer_feedback_id</t>
   </si>
   <si>
@@ -661,9 +659,6 @@
     <t>rbmalaya@fit.edu.ph</t>
   </si>
   <si>
-    <t>ECECORREL1</t>
-  </si>
-  <si>
     <t>EECORREL1</t>
   </si>
   <si>
@@ -688,9 +683,6 @@
     <t>Rona Mae</t>
   </si>
   <si>
-    <t>ECE graduate</t>
-  </si>
-  <si>
     <t>rgbabaran@gmail.com</t>
   </si>
   <si>
@@ -718,15 +710,9 @@
     <t>Mathematics ME</t>
   </si>
   <si>
-    <t>Mathematics ECE</t>
-  </si>
-  <si>
     <t>Mathematics EE</t>
   </si>
   <si>
-    <t>Hydraulics ECE</t>
-  </si>
-  <si>
     <t>Hydraulics EE</t>
   </si>
   <si>
@@ -1199,12 +1185,24 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>EEECORREL1</t>
+  </si>
+  <si>
+    <t>EEE graduate</t>
+  </si>
+  <si>
+    <t>Mathematics EEE</t>
+  </si>
+  <si>
+    <t>Hydraulics EEE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1544,7 +1542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1604,7 +1602,7 @@
         <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1614,11 +1612,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,16 +1631,16 @@
         <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1650,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -1667,7 +1665,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -1684,7 +1682,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -1701,7 +1699,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -1718,10 +1716,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>266</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1735,10 +1733,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>266</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -1752,10 +1750,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -1769,10 +1767,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1787,11 +1785,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1813,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C1" t="s">
         <v>44</v>
@@ -1828,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -1837,7 +1835,7 @@
         <v>47</v>
       </c>
       <c r="J1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1857,7 +1855,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
@@ -1866,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1898,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1912,7 +1910,7 @@
         <v>201033333</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1921,16 +1919,16 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>213</v>
+        <v>380</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1944,7 +1942,7 @@
         <v>201044444</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1953,16 +1951,16 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1970,10 +1968,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
@@ -1981,11 +1979,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1999,13 +1997,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
-        <v>94</v>
-      </c>
       <c r="C1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2019,10 +2017,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2036,10 +2034,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2053,10 +2051,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>381</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2070,10 +2068,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2087,10 +2085,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -2104,10 +2102,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2121,10 +2119,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>382</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -2138,10 +2136,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -2156,7 +2154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2175,16 +2173,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>78</v>
-      </c>
-      <c r="D1" t="s">
-        <v>79</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -2204,7 +2202,7 @@
         <v>1517968200</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2224,7 +2222,7 @@
         <v>1518073200</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2244,7 +2242,7 @@
         <v>1518174000</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2264,7 +2262,7 @@
         <v>1518238800</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2279,7 +2277,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2297,10 +2295,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -2309,7 +2307,7 @@
         <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2369,7 +2367,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2380,13 +2378,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" t="s">
         <v>249</v>
-      </c>
-      <c r="C1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2428,7 +2426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2439,13 +2437,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2487,7 +2485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2508,16 +2506,16 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
         <v>82</v>
       </c>
-      <c r="C1" t="s">
-        <v>83</v>
-      </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2525,10 +2523,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2542,10 +2540,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2559,10 +2557,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2576,10 +2574,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2594,7 +2592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2635,7 +2633,7 @@
         <v>69</v>
       </c>
       <c r="H1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2658,10 +2656,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2670,7 +2668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2721,7 +2719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2734,10 +2732,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2745,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2753,7 +2751,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2761,7 +2759,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2769,7 +2767,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2777,7 +2775,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -2786,10 +2784,10 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -2870,7 +2868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2911,10 +2909,10 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I1" t="s">
         <v>47</v>
@@ -2949,7 +2947,7 @@
         <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -2960,28 +2958,28 @@
         <v>201511438</v>
       </c>
       <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
         <v>115</v>
       </c>
-      <c r="C3" t="s">
-        <v>116</v>
-      </c>
       <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
         <v>129</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="F3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -2992,28 +2990,28 @@
         <v>201411491</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" t="s">
         <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -3024,28 +3022,28 @@
         <v>201410679</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H5" t="s">
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -3056,28 +3054,28 @@
         <v>201411851</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -3088,28 +3086,28 @@
         <v>201410215</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H7" t="s">
         <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -3120,28 +3118,28 @@
         <v>201420096</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J8">
         <v>2</v>
@@ -3152,28 +3150,28 @@
         <v>201512590</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H9" t="s">
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -3184,28 +3182,28 @@
         <v>201411823</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H10" t="s">
         <v>22</v>
       </c>
       <c r="I10" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -3216,28 +3214,28 @@
         <v>201410617</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J11">
         <v>3</v>
@@ -3248,28 +3246,28 @@
         <v>201410881</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J12">
         <v>3</v>
@@ -3280,28 +3278,28 @@
         <v>201512068</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H13" t="s">
         <v>29</v>
       </c>
       <c r="I13" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J13">
         <v>3</v>
@@ -3312,28 +3310,28 @@
         <v>201512491</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
       </c>
       <c r="I14" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J14">
         <v>3</v>
@@ -3344,28 +3342,28 @@
         <v>201510652</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H15" t="s">
         <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J15">
         <v>3</v>
@@ -3376,28 +3374,28 @@
         <v>201511230</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H16" t="s">
         <v>29</v>
       </c>
       <c r="I16" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J16">
         <v>4</v>
@@ -3408,28 +3406,28 @@
         <v>201511911</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H17" t="s">
         <v>29</v>
       </c>
       <c r="I17" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J17">
         <v>4</v>
@@ -3440,28 +3438,28 @@
         <v>201510573</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H18" t="s">
         <v>29</v>
       </c>
       <c r="I18" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J18">
         <v>4</v>
@@ -3472,28 +3470,28 @@
         <v>201512532</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H19" t="s">
         <v>29</v>
       </c>
       <c r="I19" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J19">
         <v>4</v>
@@ -3504,28 +3502,28 @@
         <v>201510186</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H20" t="s">
         <v>29</v>
       </c>
       <c r="I20" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J20">
         <v>4</v>
@@ -3533,10 +3531,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4:G7" r:id="rId3" display="adre@fit.edu.ph"/>
-    <hyperlink ref="G8:G20" r:id="rId4" display="adre@fit.edu.ph"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
+    <hyperlink ref="G4:G7" r:id="rId3" display="adre@fit.edu.ph" xr:uid="{00000000-0004-0000-1400-000002000000}"/>
+    <hyperlink ref="G8:G20" r:id="rId4" display="adre@fit.edu.ph" xr:uid="{00000000-0004-0000-1400-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
@@ -3544,7 +3542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3564,16 +3562,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
       <c r="D1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E1" t="s">
         <v>38</v>
@@ -3596,7 +3594,7 @@
         <v>1515455338</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -3622,7 +3620,7 @@
         <v>1517149393</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -3648,7 +3646,7 @@
         <v>1517152407</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -3674,7 +3672,7 @@
         <v>1517152410</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -3700,7 +3698,7 @@
         <v>1517152981</v>
       </c>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -3726,7 +3724,7 @@
         <v>1517152985</v>
       </c>
       <c r="C7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -3750,7 +3748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3765,10 +3763,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3776,7 +3774,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3785,10 +3783,10 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3805,28 +3803,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1" t="s">
         <v>255</v>
       </c>
-      <c r="B1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E1" t="s">
-        <v>260</v>
-      </c>
       <c r="F1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="G1" t="s">
         <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3834,10 +3832,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" t="s">
         <v>257</v>
-      </c>
-      <c r="C2" t="s">
-        <v>262</v>
       </c>
       <c r="D2">
         <v>1518443372</v>
@@ -3858,7 +3856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
@@ -3874,13 +3872,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3888,7 +3886,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3899,7 +3897,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3910,7 +3908,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3921,7 +3919,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3932,7 +3930,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3943,7 +3941,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3954,7 +3952,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3965,7 +3963,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3976,7 +3974,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3987,7 +3985,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3998,7 +3996,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -4009,7 +4007,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -4020,7 +4018,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -4031,7 +4029,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -4042,7 +4040,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -4053,7 +4051,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -4064,7 +4062,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -4075,7 +4073,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4086,7 +4084,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -4097,7 +4095,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -4108,7 +4106,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -4119,7 +4117,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -4130,7 +4128,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -4141,7 +4139,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -4152,7 +4150,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -4163,7 +4161,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -4174,7 +4172,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -4185,7 +4183,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -4196,7 +4194,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -4207,7 +4205,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -4218,7 +4216,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -4229,7 +4227,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -4240,7 +4238,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -4251,7 +4249,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -4262,7 +4260,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -4273,7 +4271,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -4284,7 +4282,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -4295,7 +4293,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -4306,7 +4304,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -4317,7 +4315,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -4328,7 +4326,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -4339,7 +4337,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -4350,7 +4348,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -4361,7 +4359,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -4372,7 +4370,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -4383,7 +4381,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -4394,7 +4392,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -4405,7 +4403,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -4416,7 +4414,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -4427,7 +4425,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -4438,7 +4436,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -4449,7 +4447,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -4460,7 +4458,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -4471,7 +4469,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -4482,7 +4480,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -4493,7 +4491,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -4504,7 +4502,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -4515,7 +4513,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -4526,7 +4524,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -4537,7 +4535,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -4548,7 +4546,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -4559,7 +4557,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -4570,7 +4568,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4581,7 +4579,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -4592,7 +4590,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4603,7 +4601,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -4614,7 +4612,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -4625,7 +4623,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4636,7 +4634,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -4647,7 +4645,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -4658,7 +4656,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4669,7 +4667,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4680,7 +4678,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4691,7 +4689,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -4702,7 +4700,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4713,7 +4711,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -4724,7 +4722,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4735,7 +4733,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -4746,7 +4744,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -4757,7 +4755,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -4768,7 +4766,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4779,7 +4777,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -4790,7 +4788,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -4801,7 +4799,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -4812,7 +4810,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -4823,7 +4821,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -4834,7 +4832,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -4845,7 +4843,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -4856,7 +4854,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -4868,7 +4866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4886,19 +4884,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4906,13 +4904,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E2" s="7">
         <v>2</v>
@@ -4923,13 +4921,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E3" s="6">
         <v>3</v>
@@ -4940,13 +4938,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E4" s="6">
         <v>5</v>
@@ -4957,16 +4955,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -4974,16 +4972,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -4991,16 +4989,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -5008,13 +5006,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E8" s="7">
         <v>2</v>
@@ -5025,13 +5023,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E9" s="6">
         <v>3</v>
@@ -5042,13 +5040,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E10" s="6">
         <v>5</v>
@@ -5059,16 +5057,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -5076,16 +5074,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -5093,16 +5091,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -5110,13 +5108,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
@@ -5127,13 +5125,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E15" s="6">
         <v>3</v>
@@ -5144,13 +5142,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E16" s="6">
         <v>5</v>
@@ -5161,16 +5159,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -5178,16 +5176,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -5195,16 +5193,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -5212,16 +5210,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -5229,16 +5227,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -5246,13 +5244,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E22" s="7">
         <v>2</v>
@@ -5263,13 +5261,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E23" s="6">
         <v>3</v>
@@ -5280,13 +5278,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E24" s="6">
         <v>5</v>
@@ -5297,16 +5295,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -5314,16 +5312,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -5331,16 +5329,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -5350,7 +5348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5365,10 +5363,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7417,7 +7415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7443,7 +7441,7 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -7481,11 +7479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7520,7 +7518,7 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -7532,10 +7530,10 @@
         <v>47</v>
       </c>
       <c r="J1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K1" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -7564,7 +7562,7 @@
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -7599,7 +7597,7 @@
         <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -7613,28 +7611,28 @@
         <v>201133333</v>
       </c>
       <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
         <v>85</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>86</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>266</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>89</v>
       </c>
-      <c r="H4" t="s">
-        <v>90</v>
-      </c>
       <c r="I4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -7648,28 +7646,28 @@
         <v>201144444</v>
       </c>
       <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" t="s">
         <v>103</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>104</v>
       </c>
-      <c r="H5" t="s">
-        <v>105</v>
-      </c>
       <c r="I5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -7680,10 +7678,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
@@ -7691,11 +7689,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7712,19 +7710,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" t="s">
         <v>187</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1" t="s">
         <v>188</v>
       </c>
-      <c r="C1" t="s">
-        <v>379</v>
-      </c>
-      <c r="D1" t="s">
-        <v>189</v>
-      </c>
       <c r="E1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
@@ -7733,7 +7731,7 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -7741,10 +7739,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -7767,10 +7765,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
         <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -7793,13 +7791,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C4" t="s">
         <v>204</v>
       </c>
-      <c r="C4" t="s">
-        <v>206</v>
-      </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>266</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -7819,13 +7817,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" t="s">
         <v>205</v>
       </c>
-      <c r="C5" t="s">
-        <v>207</v>
-      </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -7847,11 +7845,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7867,7 +7865,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
@@ -7885,16 +7883,16 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H1" t="s">
         <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -7902,25 +7900,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
         <v>199</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>200</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>201</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="H2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
@@ -7934,25 +7932,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" t="s">
         <v>200</v>
       </c>
-      <c r="D3" t="s">
-        <v>201</v>
-      </c>
       <c r="E3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -7966,28 +7964,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" t="s">
         <v>200</v>
       </c>
-      <c r="D4" t="s">
-        <v>201</v>
-      </c>
       <c r="E4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>266</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -7998,28 +7996,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
         <v>200</v>
       </c>
-      <c r="D5" t="s">
-        <v>201</v>
-      </c>
       <c r="E5" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F5" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -8027,10 +8025,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update dbase and controller
-UI on topic and subject area management
-on-going: putting students on sections per course.
-next: finish the ui
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" tabRatio="810" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" tabRatio="810" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="8" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="379">
   <si>
     <t>lecturer_id</t>
   </si>
@@ -1180,6 +1180,9 @@
   </si>
   <si>
     <t>subject_list_description</t>
+  </si>
+  <si>
+    <t>topic_list_description</t>
   </si>
 </sst>
 </file>
@@ -3780,10 +3783,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K18:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3791,9 +3794,10 @@
     <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="25.77734375" customWidth="1"/>
     <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>274</v>
       </c>
@@ -3803,8 +3807,11 @@
       <c r="C1" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3815,7 +3822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3826,7 +3833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3837,7 +3844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3848,7 +3855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3859,7 +3866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3870,7 +3877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3881,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3892,7 +3899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3903,7 +3910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3914,7 +3921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3925,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3936,7 +3943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3947,7 +3954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3958,7 +3965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4792,8 +4799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>